<commit_message>
mejora sustancial del codigo
</commit_message>
<xml_diff>
--- a/Web Scraping Instagram.xlsx
+++ b/Web Scraping Instagram.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc2f665d439490a3/Escritorio/Code/Artilujios/Instagram Scrapper/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_AD04E39E15F66FFC05FC9890E2E09AF7A73862CA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CDA84C2-5FC0-4473-B7A5-349E2106586D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1170" yWindow="1590" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -49,11 +55,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,7 +80,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF94E5FF"/>
+        <fgColor rgb="FF0099FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -115,17 +127,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0099FF"/>
+      <color rgb="FF3399FF"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -172,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,9 +231,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,6 +283,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,14 +476,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,21 +514,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="H2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>13</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>566</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>1080</v>
       </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>